<commit_message>
SVM classifier on normalised dataset | Added plots | Added model saving part(joblib)
</commit_message>
<xml_diff>
--- a/SVM Classifier/SVM_Results.xlsx
+++ b/SVM Classifier/SVM_Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\.1 PRML\Project_Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\.1 PRML\Project_Repo\Delete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB621CB-B556-4F14-9484-B1A1D7B80F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4928BA5-6F3A-4AF8-B9F1-33610801066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-2310" windowWidth="20730" windowHeight="11040" xr2:uid="{4B0B814F-9A33-46F3-ABEC-29DF51C59B8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="16">
   <si>
     <t>LinearSVC</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>HoG with PCA(Variance =  0.95)</t>
+  </si>
+  <si>
+    <t>Not Normalised</t>
+  </si>
+  <si>
+    <t>Normalised</t>
   </si>
 </sst>
 </file>
@@ -191,8 +197,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -202,14 +213,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7447A1F-EC7A-49F1-9E57-9C24CE5932A4}">
-  <dimension ref="B1:R27"/>
+  <dimension ref="B1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,442 +546,731 @@
     <col min="15" max="15" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+    </row>
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5">
+      <c r="D5">
         <v>11.29</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
+      <c r="D6">
         <v>35.57</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="D7">
         <v>30.77</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
         <v>31.41</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E8">
         <v>0.1</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F8" s="2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>29.8</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
         <v>29.48</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="4">
         <v>0.1</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F10" s="5">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="1" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="N11" s="1" t="s">
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="N12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
+      <c r="H13" s="1"/>
+      <c r="J13" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K13" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5" t="s">
+      <c r="N13" s="1"/>
+      <c r="P13" t="s">
         <v>6</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="Q13" t="s">
         <v>7</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="R13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5">
+      <c r="D14">
         <v>75.959999999999994</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="H13" s="4" t="s">
+      <c r="F14" s="2"/>
+      <c r="H14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5">
+      <c r="J14">
         <v>83.97</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="6"/>
-      <c r="N13" s="4" t="s">
+      <c r="L14" s="2"/>
+      <c r="N14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5">
+      <c r="P14">
         <v>26.92</v>
       </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="6"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5">
+      <c r="D15">
         <v>76.599999999999994</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="H14" s="4" t="s">
+      <c r="F15" s="2"/>
+      <c r="H15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5">
+      <c r="J15">
         <v>80.13</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
-      <c r="N14" s="4" t="s">
+      <c r="L15" s="2"/>
+      <c r="N15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5">
+      <c r="P15">
         <v>32.69</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="6"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5">
+      <c r="D16">
         <v>61.85</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="H15" s="4" t="s">
+      <c r="F16" s="2"/>
+      <c r="H16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5">
+      <c r="J16">
         <v>34.29</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="6"/>
-      <c r="N15" s="4" t="s">
+      <c r="L16" s="2"/>
+      <c r="N16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5">
+      <c r="P16">
         <v>30.77</v>
       </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="6"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="11">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
         <v>74.040000000000006</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E17">
         <v>0.1</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F17" s="2">
         <v>0.1</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="11">
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17">
         <v>38.14</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K17">
         <v>0.1</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L17" s="2">
         <v>0.1</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P16" s="11">
+      <c r="O17" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17">
         <v>31.09</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="Q17">
         <v>0.1</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="11">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
         <v>55.77</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="11">
+      <c r="F18" s="2"/>
+      <c r="H18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18">
         <v>57.37</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="6"/>
-      <c r="N17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="11">
+      <c r="L18" s="2"/>
+      <c r="N18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18">
         <v>30.77</v>
       </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="6"/>
-    </row>
-    <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="8">
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4">
         <v>75.319999999999993</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E19" s="4">
         <v>100</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F19" s="5">
         <v>1E-3</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" s="8">
+      <c r="H19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4">
         <v>77.88</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K19" s="4">
         <v>8.9</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L19" s="5">
         <v>1.2E-2</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="P18" s="8">
+      <c r="N19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="4">
         <v>29.48</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="Q19" s="4">
         <v>0.1</v>
       </c>
-      <c r="R18" s="9">
+      <c r="R19" s="5">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+    <row r="21" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" s="1"/>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>87.5</v>
+      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>80.12</v>
+      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>30.13</v>
+      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>30.45</v>
+      </c>
+      <c r="E27">
+        <v>0.1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>48.396999999999998</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>33.33</v>
+      </c>
+      <c r="E29" s="4">
+        <v>10</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="H31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="8"/>
+      <c r="N31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="8"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="J32" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" s="1"/>
+      <c r="P32" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>7</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>69.87</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="H33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>75.64</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="N33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>24.68</v>
+      </c>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="H34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>77.56</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="N34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>27.24</v>
+      </c>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>30.77</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="H35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>29.49</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="N35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P35">
+        <v>31.41</v>
+      </c>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>37.18</v>
+      </c>
+      <c r="E36">
+        <v>0.1</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36">
+        <v>29.49</v>
+      </c>
+      <c r="K36">
+        <v>0.1</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O36" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36">
+        <v>32.69</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>46.47</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="H37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>45.19</v>
+      </c>
+      <c r="L37" s="2"/>
+      <c r="N37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P37">
+        <v>33.01</v>
+      </c>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="4">
+        <v>44.87</v>
+      </c>
+      <c r="E38" s="4">
+        <v>10</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="4">
+        <v>54.17</v>
+      </c>
+      <c r="K38" s="4">
+        <v>10</v>
+      </c>
+      <c r="L38" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P38" s="4">
+        <v>37.18</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>10</v>
+      </c>
+      <c r="R38" s="5">
+        <v>1E-3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="N11:R11"/>
+  <mergeCells count="10">
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="B1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SVM Classifier : added code and results for min num. of images >=70
</commit_message>
<xml_diff>
--- a/SVM Classifier/SVM_Results.xlsx
+++ b/SVM Classifier/SVM_Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\.1 PRML\Project_Repo\Delete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\.1 PRML\Project_Repo\Face_Recognition\SVM Classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4928BA5-6F3A-4AF8-B9F1-33610801066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C239E1-0019-4CE5-85DC-CFA55E14F923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-2310" windowWidth="20730" windowHeight="11040" xr2:uid="{4B0B814F-9A33-46F3-ABEC-29DF51C59B8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
   <si>
     <t>LinearSVC</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">Polynomial Kernel </t>
   </si>
   <si>
-    <t>Tunned Hyperparameteres</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>Normalised</t>
+  </si>
+  <si>
+    <t>Accuracy(Training)</t>
+  </si>
+  <si>
+    <t>Tunned Hyperparameters</t>
   </si>
 </sst>
 </file>
@@ -204,6 +207,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -211,9 +217,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -530,747 +533,801 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7447A1F-EC7A-49F1-9E57-9C24CE5932A4}">
-  <dimension ref="B1:R38"/>
+  <dimension ref="B1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
-    <col min="15" max="15" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-    </row>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>11.29</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>35.57</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>30.77</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>31.41</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>29.8</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <v>29.48</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="I12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="O12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
-        <v>31.41</v>
-      </c>
-      <c r="E8">
-        <v>0.1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>29.8</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="K13" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="4">
-        <v>29.48</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="H12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
-      <c r="N12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="D13" t="s">
+      <c r="L13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" t="s">
+      <c r="M13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="J13" t="s">
+      <c r="O13" s="1"/>
+      <c r="Q13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" t="s">
+      <c r="S13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="P13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>7</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>75.959999999999994</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="H14" s="1" t="s">
+      <c r="G14" s="2"/>
+      <c r="I14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>83.97</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="N14" s="1" t="s">
+      <c r="M14" s="2"/>
+      <c r="O14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>26.92</v>
       </c>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>76.599999999999994</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="H15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15">
+      <c r="G15" s="2"/>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15">
         <v>80.13</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="N15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P15">
+      <c r="M15" s="2"/>
+      <c r="O15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15">
         <v>32.69</v>
       </c>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>61.85</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="H16" s="1" t="s">
+      <c r="G16" s="2"/>
+      <c r="I16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>34.29</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="N16" s="1" t="s">
+      <c r="M16" s="2"/>
+      <c r="O16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>30.77</v>
       </c>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
         <v>74.040000000000006</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.1</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0.1</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I17" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17">
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17">
         <v>38.14</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>0.1</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>0.1</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O17" t="s">
-        <v>5</v>
-      </c>
-      <c r="P17">
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17">
         <v>31.09</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>0.1</v>
       </c>
-      <c r="R17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>55.77</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="H18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18">
+      <c r="G18" s="2"/>
+      <c r="I18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18">
         <v>57.37</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="N18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P18">
+      <c r="M18" s="2"/>
+      <c r="O18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18">
         <v>30.77</v>
       </c>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4">
         <v>75.319999999999993</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>100</v>
       </c>
-      <c r="F19" s="5">
+      <c r="G19" s="5">
         <v>1E-3</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" s="4">
+      <c r="I19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="4">
         <v>77.88</v>
       </c>
-      <c r="K19" s="4">
+      <c r="L19" s="4">
         <v>8.9</v>
       </c>
-      <c r="L19" s="5">
+      <c r="M19" s="5">
         <v>1.2E-2</v>
       </c>
-      <c r="N19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P19" s="4">
+      <c r="O19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="4">
         <v>29.48</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R19" s="4">
         <v>0.1</v>
       </c>
-      <c r="R19" s="5">
+      <c r="S19" s="5">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+    <row r="21" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
         <v>87.5</v>
       </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>80.12</v>
       </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D26">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="E26">
         <v>30.13</v>
       </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>30.45</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>0.1</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28">
+        <v>0.96</v>
+      </c>
+      <c r="E28">
         <v>48.396999999999998</v>
       </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4">
         <v>33.33</v>
       </c>
-      <c r="E29" s="4">
+      <c r="F29" s="4">
         <v>10</v>
       </c>
-      <c r="F29" s="5">
+      <c r="G29" s="5">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
+    <row r="30" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="9"/>
+      <c r="I31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="H31" s="6" t="s">
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="9"/>
+      <c r="O31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="8"/>
-      <c r="N31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S31" s="9"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
         <v>6</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="J32" t="s">
+      <c r="I32" s="1"/>
+      <c r="K32" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" t="s">
         <v>6</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N32" s="1"/>
-      <c r="P32" t="s">
+      <c r="O32" s="1"/>
+      <c r="Q32" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" t="s">
         <v>6</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="S32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R32" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
         <v>69.87</v>
       </c>
-      <c r="F33" s="2"/>
-      <c r="H33" s="1" t="s">
+      <c r="G33" s="2"/>
+      <c r="I33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>75.64</v>
       </c>
-      <c r="L33" s="2"/>
-      <c r="N33" s="1" t="s">
+      <c r="M33" s="2"/>
+      <c r="O33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P33">
+      <c r="Q33">
         <v>24.68</v>
       </c>
-      <c r="R33" s="2"/>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S33" s="2"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
         <v>76.599999999999994</v>
       </c>
-      <c r="F34" s="2"/>
-      <c r="H34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J34">
+      <c r="G34" s="2"/>
+      <c r="I34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34">
         <v>77.56</v>
       </c>
-      <c r="L34" s="2"/>
-      <c r="N34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P34">
+      <c r="M34" s="2"/>
+      <c r="O34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34">
         <v>27.24</v>
       </c>
-      <c r="R34" s="2"/>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S34" s="2"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D35">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="E35">
         <v>30.77</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="H35" s="1" t="s">
+      <c r="G35" s="2"/>
+      <c r="I35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>29.49</v>
       </c>
-      <c r="L35" s="2"/>
-      <c r="N35" s="1" t="s">
+      <c r="M35" s="2"/>
+      <c r="O35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>31.41</v>
       </c>
-      <c r="R35" s="2"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S35" s="2"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
         <v>37.18</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>0.1</v>
       </c>
-      <c r="F36" s="2">
+      <c r="G36" s="2">
         <v>0.01</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36">
+      <c r="J36" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36">
         <v>29.49</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>0.1</v>
       </c>
-      <c r="L36" s="2">
+      <c r="M36" s="2">
         <v>0.01</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O36" t="s">
-        <v>5</v>
-      </c>
-      <c r="P36">
+      <c r="P36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q36">
         <v>32.69</v>
       </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-      <c r="R36" s="2">
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D37">
+        <v>0.878</v>
+      </c>
+      <c r="E37">
         <v>46.47</v>
       </c>
-      <c r="F37" s="2"/>
-      <c r="H37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37">
+      <c r="G37" s="2"/>
+      <c r="I37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37">
         <v>45.19</v>
       </c>
-      <c r="L37" s="2"/>
-      <c r="N37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P37">
+      <c r="M37" s="2"/>
+      <c r="O37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q37">
         <v>33.01</v>
       </c>
-      <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S37" s="2"/>
+    </row>
+    <row r="38" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4">
         <v>44.87</v>
       </c>
-      <c r="E38" s="4">
+      <c r="F38" s="4">
         <v>10</v>
       </c>
-      <c r="F38" s="5">
+      <c r="G38" s="5">
         <v>1E-3</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J38" s="4">
+      <c r="I38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" s="4">
         <v>54.17</v>
       </c>
-      <c r="K38" s="4">
+      <c r="L38" s="4">
         <v>10</v>
       </c>
-      <c r="L38" s="5">
+      <c r="M38" s="5">
         <v>1E-3</v>
       </c>
-      <c r="N38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P38" s="4">
+      <c r="O38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q38" s="4">
         <v>37.18</v>
       </c>
-      <c r="Q38" s="4">
+      <c r="R38" s="4">
         <v>10</v>
       </c>
-      <c r="R38" s="5">
+      <c r="S38" s="5">
         <v>1E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="O12:S12"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="B21:S21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="I31:M31"/>
+    <mergeCell ref="O31:S31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>